<commit_message>
fixed navi bar for smartphone view
</commit_message>
<xml_diff>
--- a/data/members/Others.xlsx
+++ b/data/members/Others.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yang/Documents/GitHub/CSS-Laboratory.github.io/data/members/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A27E58B-B606-4344-85FD-0DE22CE2B028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E0E694-225E-C14A-AF78-124F020607D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11400" yWindow="3960" windowWidth="27500" windowHeight="16360" xr2:uid="{0140EA53-EDB2-DD45-810D-3AF1A437EF00}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>name</t>
     <phoneticPr fontId="1"/>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>members/Mimiku.jpg</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/mimiku1210/</t>
   </si>
 </sst>
 </file>
@@ -504,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4056372-51FE-D245-9BD8-14A00DD6CD0B}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,11 +568,15 @@
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{0F498150-0A5D-5F41-AD77-5CC8DE36C9A6}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{8897F99E-9E2A-B74F-ACFE-0A1A365AD459}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>